<commit_message>
Fixed some bugs in the interface.
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/May16-forced-choice-trial.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/May16-forced-choice-trial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="7">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">forced_choice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circle</t>
   </si>
   <si>
     <t xml:space="preserve">5KHz</t>
@@ -80,6 +77,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -100,7 +98,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -189,11 +186,11 @@
   </sheetPr>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -291,7 +288,7 @@
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -319,7 +316,7 @@
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -330,7 +327,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -358,7 +355,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -389,7 +386,7 @@
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -403,7 +400,7 @@
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -428,7 +425,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -459,7 +456,7 @@
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -512,7 +509,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -540,7 +537,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -613,8 +610,8 @@
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
+      <c r="B31" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -631,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
@@ -641,11 +638,11 @@
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
@@ -655,25 +652,25 @@
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
@@ -687,21 +684,21 @@
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>5</v>
@@ -711,11 +708,11 @@
       <c r="A38" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
@@ -725,53 +722,53 @@
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
@@ -781,11 +778,11 @@
       <c r="A43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>5</v>
@@ -799,35 +796,35 @@
         <v>3</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
@@ -837,11 +834,11 @@
       <c r="A47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>5</v>
@@ -851,11 +848,11 @@
       <c r="A48" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>5</v>
@@ -865,11 +862,11 @@
       <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>5</v>
@@ -879,25 +876,25 @@
       <c r="A50" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>5</v>
@@ -907,11 +904,11 @@
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>5</v>
@@ -925,21 +922,21 @@
         <v>2</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>5</v>
@@ -949,11 +946,11 @@
       <c r="A55" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>5</v>
@@ -963,25 +960,25 @@
       <c r="A56" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>5</v>
@@ -991,39 +988,39 @@
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>5</v>
@@ -1033,105 +1030,103 @@
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
-      <c r="B66" s="5"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
-      <c r="B67" s="5"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
-      <c r="B68" s="5"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
-      <c r="B71" s="5"/>
+      <c r="B71" s="2"/>
       <c r="C71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
-      <c r="B73" s="5"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
-      <c r="B74" s="5"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
-      <c r="B77" s="5"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
-      <c r="B78" s="5"/>
+      <c r="B78" s="2"/>
       <c r="C78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5"/>
+      <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="1"/>
     </row>

</xml_diff>